<commit_message>
ANV - 20220330 - Add the updated report workflow
</commit_message>
<xml_diff>
--- a/TH02/Data/Config.xlsx
+++ b/TH02/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ansverma\Desktop\Desktop\Project\ADEO_Laptop29_6_21\Adeo\Project\ISOCEL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ansverma\Desktop\Desktop\Project\ADEO_Laptop29_6_21\Adeo\Project\ISOCEL\Project\TestCase1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33BEA3E9-8DF3-4021-88DA-BA63A7C1EEEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0012F8F-B405-494B-93FE-891E7ED43674}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -185,6 +185,33 @@
   </si>
   <si>
     <t>TH02_Alice_isocel_Credential</t>
+  </si>
+  <si>
+    <t>FileReport</t>
+  </si>
+  <si>
+    <t>Variation Data\TH02.xlsx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This pathis for test case excel file. </t>
+  </si>
+  <si>
+    <t>Testcase1SheetName</t>
+  </si>
+  <si>
+    <t>010_Create_dossier_d'offre</t>
+  </si>
+  <si>
+    <t>020_Valuation_of_the_articles</t>
+  </si>
+  <si>
+    <t>Testcase2SheetName</t>
+  </si>
+  <si>
+    <t>Sheet name of the testcase 1 for THo2 file</t>
+  </si>
+  <si>
+    <t>Sheet name of the testcase 2 for THo2 file</t>
   </si>
 </sst>
 </file>
@@ -595,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -686,9 +713,39 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
@@ -2805,8 +2862,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>